<commit_message>
update and some formatting
</commit_message>
<xml_diff>
--- a/run_cloud_experiments/input/300_gridConnections/db_backboneConfig_300.xlsx
+++ b/run_cloud_experiments/input/300_gridConnections/db_backboneConfig_300.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\WIES4\Documents\00projecten\HOLON\HOLON-anylogic\run_cloud_experiments\input\300_gridConnections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\WIES4\Documents\00projecten\HOLON\HOLON-cloudclient\run_cloud_experiments\input\300_gridConnections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB80B11B-6EE0-4AA3-8AB1-9CB33884B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F759DB9-FDC6-4F5A-9518-695D7B53941B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="4" xr2:uid="{C61B0771-0652-4F35-8DF1-D2D550B8F66D}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -2521,13 +2521,14 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -17668,7 +17669,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -17725,7 +17726,7 @@
         <v>44</v>
       </c>
       <c r="G2" s="1">
-        <v>8000</v>
+        <v>0</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -17751,7 +17752,7 @@
         <v>44</v>
       </c>
       <c r="G3" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -17777,7 +17778,7 @@
         <v>46</v>
       </c>
       <c r="G4" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -17803,7 +17804,7 @@
         <v>46</v>
       </c>
       <c r="G5" s="1">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -17829,7 +17830,7 @@
         <v>47</v>
       </c>
       <c r="G6" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -17855,7 +17856,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -17881,7 +17882,7 @@
         <v>460</v>
       </c>
       <c r="G8" s="1">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -17907,7 +17908,7 @@
         <v>460</v>
       </c>
       <c r="G9" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -17933,7 +17934,7 @@
         <v>461</v>
       </c>
       <c r="G10" s="1">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -17959,7 +17960,7 @@
         <v>461</v>
       </c>
       <c r="G11" s="1">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -17985,7 +17986,7 @@
         <v>462</v>
       </c>
       <c r="G12" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -18011,7 +18012,7 @@
         <v>462</v>
       </c>
       <c r="G13" s="1">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>

</xml_diff>